<commit_message>
testando algoritmos de feature selection (deu certo)
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/rodada1/params.xlsx
+++ b/models/dissertation-model/modelo-R/rodada1/params.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId2"/>
@@ -519,7 +519,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -529,10 +529,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -567,23 +563,23 @@
   </sheetPr>
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="46.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +649,7 @@
       </c>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
-      <c r="L2" s="3" t="n">
+      <c r="L2" s="1" t="n">
         <f aca="false">C2=D2</f>
         <v>0</v>
       </c>
@@ -688,7 +684,7 @@
       </c>
       <c r="J3" s="0"/>
       <c r="K3" s="0"/>
-      <c r="L3" s="3" t="n">
+      <c r="L3" s="1" t="n">
         <f aca="false">C3=D3</f>
         <v>1</v>
       </c>
@@ -721,7 +717,7 @@
       </c>
       <c r="J4" s="0"/>
       <c r="K4" s="0"/>
-      <c r="L4" s="3" t="n">
+      <c r="L4" s="1" t="n">
         <f aca="false">C4=D4</f>
         <v>1</v>
       </c>
@@ -758,7 +754,7 @@
       </c>
       <c r="J5" s="0"/>
       <c r="K5" s="0"/>
-      <c r="L5" s="3" t="n">
+      <c r="L5" s="1" t="n">
         <f aca="false">C5=D5</f>
         <v>1</v>
       </c>
@@ -794,7 +790,7 @@
       <c r="K6" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="L6" s="3" t="n">
+      <c r="L6" s="1" t="n">
         <f aca="false">C6=D6</f>
         <v>0</v>
       </c>
@@ -826,7 +822,7 @@
       </c>
       <c r="J7" s="0"/>
       <c r="K7" s="0"/>
-      <c r="L7" s="3" t="n">
+      <c r="L7" s="1" t="n">
         <f aca="false">C7=D7</f>
         <v>1</v>
       </c>
@@ -856,7 +852,7 @@
       </c>
       <c r="J8" s="0"/>
       <c r="K8" s="0"/>
-      <c r="L8" s="3" t="n">
+      <c r="L8" s="1" t="n">
         <f aca="false">C8=D8</f>
         <v>1</v>
       </c>
@@ -892,7 +888,7 @@
       <c r="K9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="L9" s="1" t="n">
         <f aca="false">C9=D9</f>
         <v>0</v>
       </c>
@@ -922,7 +918,7 @@
       </c>
       <c r="J10" s="0"/>
       <c r="K10" s="0"/>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="1" t="n">
         <f aca="false">C10=D10</f>
         <v>1</v>
       </c>
@@ -954,7 +950,7 @@
       </c>
       <c r="J11" s="0"/>
       <c r="K11" s="0"/>
-      <c r="L11" s="3" t="n">
+      <c r="L11" s="1" t="n">
         <f aca="false">C11=D11</f>
         <v>1</v>
       </c>
@@ -986,7 +982,7 @@
       </c>
       <c r="J12" s="0"/>
       <c r="K12" s="0"/>
-      <c r="L12" s="3" t="n">
+      <c r="L12" s="1" t="n">
         <f aca="false">C12=D12</f>
         <v>1</v>
       </c>
@@ -1018,7 +1014,7 @@
       </c>
       <c r="J13" s="0"/>
       <c r="K13" s="0"/>
-      <c r="L13" s="3" t="n">
+      <c r="L13" s="1" t="n">
         <f aca="false">C13=D13</f>
         <v>1</v>
       </c>
@@ -1050,7 +1046,7 @@
       </c>
       <c r="J14" s="0"/>
       <c r="K14" s="0"/>
-      <c r="L14" s="3" t="n">
+      <c r="L14" s="1" t="n">
         <f aca="false">C14=D14</f>
         <v>1</v>
       </c>
@@ -1083,7 +1079,7 @@
       <c r="K15" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="L15" s="3" t="n">
+      <c r="L15" s="1" t="n">
         <f aca="false">C15=D15</f>
         <v>0</v>
       </c>
@@ -1114,7 +1110,7 @@
       </c>
       <c r="J16" s="0"/>
       <c r="K16" s="0"/>
-      <c r="L16" s="3" t="n">
+      <c r="L16" s="1" t="n">
         <f aca="false">C16=D16</f>
         <v>1</v>
       </c>
@@ -1147,7 +1143,7 @@
       <c r="K17" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L17" s="3" t="n">
+      <c r="L17" s="1" t="n">
         <f aca="false">C17=D17</f>
         <v>0</v>
       </c>
@@ -1178,7 +1174,7 @@
       </c>
       <c r="J18" s="0"/>
       <c r="K18" s="0"/>
-      <c r="L18" s="3" t="n">
+      <c r="L18" s="1" t="n">
         <f aca="false">C18=D18</f>
         <v>1</v>
       </c>
@@ -1209,7 +1205,7 @@
       </c>
       <c r="J19" s="0"/>
       <c r="K19" s="0"/>
-      <c r="L19" s="3" t="n">
+      <c r="L19" s="1" t="n">
         <f aca="false">C19=D19</f>
         <v>1</v>
       </c>
@@ -1239,7 +1235,7 @@
       </c>
       <c r="J20" s="0"/>
       <c r="K20" s="0"/>
-      <c r="L20" s="3" t="n">
+      <c r="L20" s="1" t="n">
         <f aca="false">C20=D20</f>
         <v>0</v>
       </c>
@@ -1272,7 +1268,7 @@
       <c r="K21" s="1" t="n">
         <v>-4</v>
       </c>
-      <c r="L21" s="3" t="n">
+      <c r="L21" s="1" t="n">
         <f aca="false">C21=D21</f>
         <v>0</v>
       </c>
@@ -1298,7 +1294,7 @@
       </c>
       <c r="J22" s="0"/>
       <c r="K22" s="0"/>
-      <c r="L22" s="3" t="n">
+      <c r="L22" s="1" t="n">
         <f aca="false">C22=D22</f>
         <v>0</v>
       </c>
@@ -1326,7 +1322,7 @@
       </c>
       <c r="J23" s="0"/>
       <c r="K23" s="0"/>
-      <c r="L23" s="3" t="n">
+      <c r="L23" s="1" t="n">
         <f aca="false">C23=D23</f>
         <v>1</v>
       </c>
@@ -1358,7 +1354,7 @@
       <c r="K24" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L24" s="3" t="n">
+      <c r="L24" s="1" t="n">
         <f aca="false">C24=D24</f>
         <v>0</v>
       </c>
@@ -1384,7 +1380,7 @@
       </c>
       <c r="J25" s="0"/>
       <c r="K25" s="0"/>
-      <c r="L25" s="3" t="n">
+      <c r="L25" s="1" t="n">
         <f aca="false">C25=D25</f>
         <v>1</v>
       </c>
@@ -1412,7 +1408,7 @@
       </c>
       <c r="J26" s="0"/>
       <c r="K26" s="0"/>
-      <c r="L26" s="3" t="n">
+      <c r="L26" s="1" t="n">
         <f aca="false">C26=D26</f>
         <v>1</v>
       </c>
@@ -1442,13 +1438,13 @@
       <c r="K27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L27" s="3" t="n">
+      <c r="L27" s="1" t="n">
         <f aca="false">C27=D27</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1468,7 +1464,7 @@
       </c>
       <c r="J28" s="0"/>
       <c r="K28" s="0"/>
-      <c r="L28" s="3" t="n">
+      <c r="L28" s="1" t="n">
         <f aca="false">C28=D28</f>
         <v>1</v>
       </c>
@@ -1489,16 +1485,16 @@
       <c r="E29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="5" t="n">
+      <c r="I29" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="J29" s="5" t="n">
+      <c r="J29" s="4" t="n">
         <v>0.6</v>
       </c>
-      <c r="K29" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L29" s="3" t="n">
+      <c r="K29" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1" t="n">
         <f aca="false">C29=D29</f>
         <v>0</v>
       </c>
@@ -1523,7 +1519,7 @@
       </c>
       <c r="J30" s="0"/>
       <c r="K30" s="0"/>
-      <c r="L30" s="3" t="n">
+      <c r="L30" s="1" t="n">
         <f aca="false">C30=D30</f>
         <v>0</v>
       </c>
@@ -1549,7 +1545,7 @@
       </c>
       <c r="J31" s="0"/>
       <c r="K31" s="0"/>
-      <c r="L31" s="3" t="n">
+      <c r="L31" s="1" t="n">
         <f aca="false">C31=D31</f>
         <v>1</v>
       </c>
@@ -1577,7 +1573,7 @@
       </c>
       <c r="J32" s="0"/>
       <c r="K32" s="0"/>
-      <c r="L32" s="3" t="n">
+      <c r="L32" s="1" t="n">
         <f aca="false">C32=D32</f>
         <v>1</v>
       </c>
@@ -1605,7 +1601,7 @@
       </c>
       <c r="J33" s="0"/>
       <c r="K33" s="0"/>
-      <c r="L33" s="3" t="n">
+      <c r="L33" s="1" t="n">
         <f aca="false">C33=D33</f>
         <v>1</v>
       </c>
@@ -1635,7 +1631,7 @@
       <c r="K34" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L34" s="3" t="n">
+      <c r="L34" s="1" t="n">
         <f aca="false">C34=D34</f>
         <v>0</v>
       </c>
@@ -1666,7 +1662,7 @@
       <c r="K35" s="1" t="n">
         <v>0.25</v>
       </c>
-      <c r="L35" s="3" t="n">
+      <c r="L35" s="1" t="n">
         <f aca="false">C35=D35</f>
         <v>0</v>
       </c>
@@ -1696,7 +1692,7 @@
       <c r="K36" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L36" s="3" t="n">
+      <c r="L36" s="1" t="n">
         <f aca="false">C36=D36</f>
         <v>0</v>
       </c>
@@ -1719,7 +1715,7 @@
       <c r="I37" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="L37" s="3" t="n">
+      <c r="L37" s="1" t="n">
         <f aca="false">C37=D37</f>
         <v>1</v>
       </c>
@@ -1743,17 +1739,17 @@
   </sheetPr>
   <dimension ref="A1:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.45408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.56122448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1776,13 +1772,13 @@
       </c>
       <c r="B2" s="1" t="str">
         <f aca="false">"C."&amp;C2&amp;"-."&amp;D2</f>
-        <v>C.1-.0,3</v>
+        <v>C.1-.0,5</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1792,84 +1788,19 @@
       </c>
       <c r="B3" s="1" t="str">
         <f aca="false">"C."&amp;C3&amp;"-."&amp;D3</f>
-        <v>C.1-.0,5</v>
+        <v>C.2-.0,5</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="1" t="n">
-        <f aca="false">D2+0.2</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <f aca="false">A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="str">
-        <f aca="false">"C."&amp;C4&amp;"-."&amp;D4</f>
-        <v>C.1-.0,7</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <f aca="false">D3+0.2</f>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <f aca="false">A4+1</f>
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="str">
-        <f aca="false">"C."&amp;C5&amp;"-."&amp;D5</f>
-        <v>C.2-.0,3</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <f aca="false">D2</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <f aca="false">A5+1</f>
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="str">
-        <f aca="false">"C."&amp;C6&amp;"-."&amp;D6</f>
-        <v>C.2-.0,5</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <f aca="false">D3</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <f aca="false">A6+1</f>
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="str">
-        <f aca="false">"C."&amp;C7&amp;"-."&amp;D7</f>
-        <v>C.2-.0,7</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <f aca="false">D4</f>
-        <v>0.7</v>
-      </c>
-    </row>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1897,12 +1828,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>103</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -1947,11 +1875,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="25.3775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
alterações no código para calibracao
</commit_message>
<xml_diff>
--- a/models/dissertation-model/modelo-R/rodada1/params.xlsx
+++ b/models/dissertation-model/modelo-R/rodada1/params.xlsx
@@ -531,7 +531,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -561,12 +561,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <u val="single"/>
@@ -625,7 +619,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -646,10 +640,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -658,7 +648,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -687,21 +677,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="55.0765306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="5.10204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.9438775510204"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.2755102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="7.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1023" min="14" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="7.29081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,7 +749,7 @@
         <f aca="false">IF(I2="Incerto",MAX(G2,J2-(ABS(F2*J2))),J2)</f>
         <v>0.5</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="2" t="n">
         <f aca="false">IF(I2="Incerto",MIN(H2,J2+(ABS(F2*J2))),J2)</f>
         <v>1.5</v>
       </c>
@@ -802,7 +792,7 @@
         <f aca="false">IF(I3="Incerto",MAX(G3,J3-(ABS(F3*J3))),J3)</f>
         <v>0.04</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="2" t="n">
         <f aca="false">IF(I3="Incerto",MIN(H3,J3+(ABS(F3*J3))),J3)</f>
         <v>0.04</v>
       </c>
@@ -845,7 +835,7 @@
         <f aca="false">IF(I4="Incerto",MAX(G4,J4-(ABS(F4*J4))),J4)</f>
         <v>0.25</v>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="2" t="n">
         <f aca="false">IF(I4="Incerto",MIN(H4,J4+(ABS(F4*J4))),J4)</f>
         <v>0.25</v>
       </c>
@@ -888,7 +878,7 @@
         <f aca="false">IF(I5="Incerto",MAX(G5,J5-(ABS(F5*J5))),J5)</f>
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="2" t="n">
         <f aca="false">IF(I5="Incerto",MIN(H5,J5+(ABS(F5*J5))),J5)</f>
         <v>1</v>
       </c>
@@ -931,7 +921,7 @@
         <f aca="false">IF(I6="Incerto",MAX(G6,J6-(ABS(F6*J6))),J6)</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="2" t="n">
         <f aca="false">IF(I6="Incerto",MIN(H6,J6+(ABS(F6*J6))),J6)</f>
         <v>0.5</v>
       </c>
@@ -979,7 +969,7 @@
         <f aca="false">IF(I7="Incerto",MAX(G7,J7-(ABS(F7*J7))),J7)</f>
         <v>0.025</v>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="2" t="n">
         <f aca="false">IF(I7="Incerto",MIN(H7,J7+(ABS(F7*J7))),J7)</f>
         <v>0.075</v>
       </c>
@@ -1022,7 +1012,7 @@
         <f aca="false">IF(I8="Incerto",MAX(G8,J8-(ABS(F8*J8))),J8)</f>
         <v>200000</v>
       </c>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="2" t="n">
         <f aca="false">IF(I8="Incerto",MIN(H8,J8+(ABS(F8*J8))),J8)</f>
         <v>200000</v>
       </c>
@@ -1065,7 +1055,7 @@
         <f aca="false">IF(I9="Incerto",MAX(G9,J9-(ABS(F9*J9))),J9)</f>
         <v>0.1</v>
       </c>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="2" t="n">
         <f aca="false">IF(I9="Incerto",MIN(H9,J9+(ABS(F9*J9))),J9)</f>
         <v>0.3</v>
       </c>
@@ -1112,7 +1102,7 @@
         <f aca="false">IF(I10="Incerto",MAX(G10,J10-(ABS(F10*J10))),J10)</f>
         <v>50000</v>
       </c>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="2" t="n">
         <f aca="false">IF(I10="Incerto",MIN(H10,J10+(ABS(F10*J10))),J10)</f>
         <v>50000</v>
       </c>
@@ -1157,7 +1147,7 @@
         <f aca="false">IF(I11="Incerto",MAX(G11,J11-(ABS(F11*J11))),J11)</f>
         <v>0.0005</v>
       </c>
-      <c r="D11" s="5" t="n">
+      <c r="D11" s="2" t="n">
         <f aca="false">IF(I11="Incerto",MIN(H11,J11+(ABS(F11*J11))),J11)</f>
         <v>0.0015</v>
       </c>
@@ -1200,7 +1190,7 @@
         <f aca="false">IF(I12="Incerto",MAX(G12,J12-(ABS(F12*J12))),J12)</f>
         <v>0.5</v>
       </c>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="2" t="n">
         <f aca="false">IF(I12="Incerto",MIN(H12,J12+(ABS(F12*J12))),J12)</f>
         <v>1.5</v>
       </c>
@@ -1243,7 +1233,7 @@
         <f aca="false">IF(I13="Incerto",MAX(G13,J13-(ABS(F13*J13))),J13)</f>
         <v>1000000</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="2" t="n">
         <f aca="false">IF(I13="Incerto",MIN(H13,J13+(ABS(F13*J13))),J13)</f>
         <v>1000000</v>
       </c>
@@ -1289,7 +1279,7 @@
         <f aca="false">IF(I14="Incerto",MAX(G14,J14-(ABS(F14*J14))),J14)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="5" t="n">
+      <c r="D14" s="2" t="n">
         <f aca="false">IF(I14="Incerto",MIN(H14,J14+(ABS(F14*J14))),J14)</f>
         <v>0</v>
       </c>
@@ -1330,7 +1320,7 @@
         <f aca="false">IF(I15="Incerto",MAX(G15,J15-(ABS(F15*J15))),J15)</f>
         <v>0.25</v>
       </c>
-      <c r="D15" s="5" t="n">
+      <c r="D15" s="2" t="n">
         <f aca="false">IF(I15="Incerto",MIN(H15,J15+(ABS(F15*J15))),J15)</f>
         <v>0.375</v>
       </c>
@@ -1377,7 +1367,7 @@
         <f aca="false">IF(I16="Incerto",MAX(G16,J16-(ABS(F16*J16))),J16)</f>
         <v>1</v>
       </c>
-      <c r="D16" s="5" t="n">
+      <c r="D16" s="2" t="n">
         <f aca="false">IF(I16="Incerto",MIN(H16,J16+(ABS(F16*J16))),J16)</f>
         <v>1</v>
       </c>
@@ -1420,7 +1410,7 @@
         <f aca="false">IF(I17="Incerto",MAX(G17,J17-(ABS(F17*J17))),J17)</f>
         <v>0.5</v>
       </c>
-      <c r="D17" s="5" t="n">
+      <c r="D17" s="2" t="n">
         <f aca="false">IF(I17="Incerto",MIN(H17,J17+(ABS(F17*J17))),J17)</f>
         <v>1.5</v>
       </c>
@@ -1467,7 +1457,7 @@
         <f aca="false">IF(I18="Incerto",MAX(G18,J18-(ABS(F18*J18))),J18)</f>
         <v>1</v>
       </c>
-      <c r="D18" s="5" t="n">
+      <c r="D18" s="2" t="n">
         <f aca="false">IF(I18="Incerto",MIN(H18,J18+(ABS(F18*J18))),J18)</f>
         <v>1</v>
       </c>
@@ -1510,7 +1500,7 @@
         <f aca="false">IF(I19="Incerto",MAX(G19,J19-(ABS(F19*J19))),J19)</f>
         <v>0.25</v>
       </c>
-      <c r="D19" s="5" t="n">
+      <c r="D19" s="2" t="n">
         <f aca="false">IF(I19="Incerto",MIN(H19,J19+(ABS(F19*J19))),J19)</f>
         <v>0.25</v>
       </c>
@@ -1553,7 +1543,7 @@
         <f aca="false">IF(I20="Incerto",MAX(G20,J20-(ABS(F20*J20))),J20)</f>
         <v>-6</v>
       </c>
-      <c r="D20" s="5" t="n">
+      <c r="D20" s="2" t="n">
         <f aca="false">IF(I20="Incerto",MIN(H20,J20+(ABS(F20*J20))),J20)</f>
         <v>-2</v>
       </c>
@@ -1596,7 +1586,7 @@
         <f aca="false">IF(I21="Incerto",MAX(G21,J21-(ABS(F21*J21))),J21)</f>
         <v>-12</v>
       </c>
-      <c r="D21" s="5" t="n">
+      <c r="D21" s="2" t="n">
         <f aca="false">IF(I21="Incerto",MIN(H21,J21+(ABS(F21*J21))),J21)</f>
         <v>-4</v>
       </c>
@@ -1643,7 +1633,7 @@
         <f aca="false">IF(I22="Incerto",MAX(G22,J22-(ABS(F22*J22))),J22)</f>
         <v>0.5</v>
       </c>
-      <c r="D22" s="5" t="n">
+      <c r="D22" s="2" t="n">
         <f aca="false">IF(I22="Incerto",MIN(H22,J22+(ABS(F22*J22))),J22)</f>
         <v>1</v>
       </c>
@@ -1686,7 +1676,7 @@
         <f aca="false">IF(H23="Incerto",MAX(G23,J23-(ABS(F23*J23))),J23)</f>
         <v>100000</v>
       </c>
-      <c r="D23" s="5" t="n">
+      <c r="D23" s="2" t="n">
         <f aca="false">IF(H23="Incerto",MIN(G23,J23+(ABS(F23*J23))),J23)</f>
         <v>100000</v>
       </c>
@@ -1732,7 +1722,7 @@
         <f aca="false">IF(I24="Incerto",MAX(G24,J24-(ABS(F24*J24))),J24)</f>
         <v>1</v>
       </c>
-      <c r="D24" s="5" t="n">
+      <c r="D24" s="2" t="n">
         <f aca="false">IF(I24="Incerto",MIN(H24,J24+(ABS(F24*J24))),J24)</f>
         <v>3</v>
       </c>
@@ -1781,7 +1771,7 @@
         <f aca="false">IF(I25="Incerto",MAX(G25,J25-(ABS(F25*J25))),J25)</f>
         <v>200000</v>
       </c>
-      <c r="D25" s="5" t="n">
+      <c r="D25" s="2" t="n">
         <f aca="false">IF(I25="Incerto",MIN(H25,J25+(ABS(F25*J25))),J25)</f>
         <v>200000</v>
       </c>
@@ -1826,7 +1816,7 @@
         <f aca="false">IF(I26="Incerto",MAX(G26,J26-(ABS(F26*J26))),J26)</f>
         <v>0.1</v>
       </c>
-      <c r="D26" s="5" t="n">
+      <c r="D26" s="2" t="n">
         <f aca="false">IF(I26="Incerto",MIN(H26,J26+(ABS(F26*J26))),J26)</f>
         <v>0.3</v>
       </c>
@@ -1869,7 +1859,7 @@
         <f aca="false">IF(I27="Incerto",MAX(G27,J27-(ABS(F27*J27))),J27)</f>
         <v>0.5</v>
       </c>
-      <c r="D27" s="5" t="n">
+      <c r="D27" s="2" t="n">
         <f aca="false">IF(I27="Incerto",MIN(H27,J27+(ABS(F27*J27))),J27)</f>
         <v>1</v>
       </c>
@@ -1906,7 +1896,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>78</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1916,7 +1906,7 @@
         <f aca="false">IF(I28="Incerto",MAX(G28,J28-(ABS(F28*J28))),J28)</f>
         <v>50</v>
       </c>
-      <c r="D28" s="5" t="n">
+      <c r="D28" s="2" t="n">
         <f aca="false">IF(I28="Incerto",MIN(H28,J28+(ABS(F28*J28))),J28)</f>
         <v>50</v>
       </c>
@@ -1962,7 +1952,7 @@
         <f aca="false">IF(I29="Incerto",MAX(G29,J29-(ABS(F29*J29))),J29)</f>
         <v>0.25</v>
       </c>
-      <c r="D29" s="5" t="n">
+      <c r="D29" s="2" t="n">
         <f aca="false">IF(I29="Incerto",MIN(H29,J29+(ABS(F29*J29))),J29)</f>
         <v>0.75</v>
       </c>
@@ -1984,13 +1974,13 @@
       <c r="J29" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="K29" s="7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L29" s="7" t="n">
+      <c r="K29" s="6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L29" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="M29" s="7" t="n">
+      <c r="M29" s="6" t="n">
         <v>1</v>
       </c>
       <c r="N29" s="1" t="n">
@@ -2009,7 +1999,7 @@
         <f aca="false">IF(I30="Incerto",MAX(G30,J30-(ABS(F30*J30))),J30)</f>
         <v>0.25</v>
       </c>
-      <c r="D30" s="5" t="n">
+      <c r="D30" s="2" t="n">
         <f aca="false">IF(I30="Incerto",MIN(H30,J30+(ABS(F30*J30))),J30)</f>
         <v>0.75</v>
       </c>
@@ -2050,7 +2040,7 @@
         <f aca="false">IF(I31="Incerto",MAX(G31,J31-(ABS(F31*J31))),J31)</f>
         <v>1</v>
       </c>
-      <c r="D31" s="5" t="n">
+      <c r="D31" s="2" t="n">
         <f aca="false">IF(I31="Incerto",MIN(H31,J31+(ABS(F31*J31))),J31)</f>
         <v>1</v>
       </c>
@@ -2091,7 +2081,7 @@
         <f aca="false">IF(I32="Incerto",MAX(G32,J32-(ABS(F32*J32))),J32)</f>
         <v>0.25</v>
       </c>
-      <c r="D32" s="5" t="n">
+      <c r="D32" s="2" t="n">
         <f aca="false">IF(I32="Incerto",MIN(H32,J32+(ABS(F32*J32))),J32)</f>
         <v>0.25</v>
       </c>
@@ -2134,7 +2124,7 @@
         <f aca="false">IF(I33="Incerto",MAX(G33,J33-(ABS(F33*J33))),J33)</f>
         <v>0.25</v>
       </c>
-      <c r="D33" s="5" t="n">
+      <c r="D33" s="2" t="n">
         <f aca="false">IF(I33="Incerto",MIN(H33,J33+(ABS(F33*J33))),J33)</f>
         <v>0.25</v>
       </c>
@@ -2177,7 +2167,7 @@
         <f aca="false">IF(I34="Incerto",MAX(G34,J34-(ABS(F34*J34))),J34)</f>
         <v>0.5</v>
       </c>
-      <c r="D34" s="5" t="n">
+      <c r="D34" s="2" t="n">
         <f aca="false">IF(I34="Incerto",MIN(H34,J34+(ABS(F34*J34))),J34)</f>
         <v>1.5</v>
       </c>
@@ -2225,7 +2215,7 @@
         <f aca="false">IF(I35="Incerto",MAX(G35,J35-(ABS(F35*J35))),J35)</f>
         <v>0.125</v>
       </c>
-      <c r="D35" s="5" t="n">
+      <c r="D35" s="2" t="n">
         <f aca="false">IF(I35="Incerto",MIN(H35,J35+(ABS(F35*J35))),J35)</f>
         <v>0.375</v>
       </c>
@@ -2273,7 +2263,7 @@
         <f aca="false">IF(I36="Incerto",MAX(G36,J36-(ABS(F36*J36))),J36)</f>
         <v>-0.15</v>
       </c>
-      <c r="D36" s="5" t="n">
+      <c r="D36" s="2" t="n">
         <f aca="false">IF(I36="Incerto",MIN(H36,J36+(ABS(F36*J36))),J36)</f>
         <v>-0.05</v>
       </c>
@@ -2320,7 +2310,7 @@
         <f aca="false">IF(I37="Incerto",MAX(G37,J37-(ABS(F37*J37))),J37)</f>
         <v>0</v>
       </c>
-      <c r="D37" s="5" t="n">
+      <c r="D37" s="2" t="n">
         <f aca="false">IF(I37="Incerto",MIN(H37,J37+(ABS(F37*J37))),J37)</f>
         <v>0</v>
       </c>
@@ -2361,7 +2351,7 @@
         <f aca="false">IF(I38="Incerto",MAX(G38,J38-(ABS(F38*J38))),J38)</f>
         <v>1</v>
       </c>
-      <c r="D38" s="5" t="n">
+      <c r="D38" s="2" t="n">
         <f aca="false">IF(I38="Incerto",MIN(H38,J38+(ABS(F38*J38))),J38)</f>
         <v>1</v>
       </c>
@@ -2398,7 +2388,7 @@
         <f aca="false">IF(I39="Incerto",MAX(G39,J39-(ABS(F39*J39))),J39)</f>
         <v>0.0005</v>
       </c>
-      <c r="D39" s="5" t="n">
+      <c r="D39" s="2" t="n">
         <f aca="false">IF(I39="Incerto",MIN(H39,J39+(ABS(F39*J39))),J39)</f>
         <v>0.0015</v>
       </c>
@@ -2435,7 +2425,7 @@
         <f aca="false">IF(I40="Incerto",MAX(G40,J40-(ABS(F40*J40))),J40)</f>
         <v>2</v>
       </c>
-      <c r="D40" s="5" t="n">
+      <c r="D40" s="2" t="n">
         <f aca="false">IF(I40="Incerto",MIN(H40,J40+(ABS(F40*J40))),J40)</f>
         <v>6</v>
       </c>
@@ -2473,7 +2463,7 @@
         <f aca="false">IF(I41="Incerto",MAX(G41,J41-(ABS(F41*J41))),J41)</f>
         <v>50000</v>
       </c>
-      <c r="D41" s="5" t="n">
+      <c r="D41" s="2" t="n">
         <f aca="false">IF(I41="Incerto",MIN(H41,J41+(ABS(F41*J41))),J41)</f>
         <v>150000</v>
       </c>
@@ -2512,7 +2502,7 @@
         <f aca="false">IF(I42="Incerto",MAX(G42,J42-(ABS(F42*J42))),J42)</f>
         <v>1</v>
       </c>
-      <c r="D42" s="5" t="n">
+      <c r="D42" s="2" t="n">
         <f aca="false">IF(I42="Incerto",MIN(H42,J42+(ABS(F42*J42))),J42)</f>
         <v>3</v>
       </c>
@@ -2551,7 +2541,7 @@
         <f aca="false">IF(I43="Incerto",MAX(G43,J43-(ABS(F43*J43))),J43)</f>
         <v>0.2</v>
       </c>
-      <c r="D43" s="5" t="n">
+      <c r="D43" s="2" t="n">
         <f aca="false">IF(I43="Incerto",MIN(H43,J43+(ABS(F43*J43))),J43)</f>
         <v>0.6</v>
       </c>
@@ -2589,7 +2579,7 @@
         <f aca="false">IF(I44="Incerto",MAX(G44,J44-(ABS(F44*J44))),J44)</f>
         <v>18</v>
       </c>
-      <c r="D44" s="5" t="n">
+      <c r="D44" s="2" t="n">
         <f aca="false">IF(I44="Incerto",MIN(H44,J44+(ABS(F44*J44))),J44)</f>
         <v>18</v>
       </c>
@@ -2628,7 +2618,7 @@
         <f aca="false">IF(I45="Incerto",MAX(G45,J45-(ABS(F45*J45))),J45)</f>
         <v>5</v>
       </c>
-      <c r="D45" s="5" t="n">
+      <c r="D45" s="2" t="n">
         <f aca="false">IF(I45="Incerto",MIN(H45,J45+(ABS(F45*J45))),J45)</f>
         <v>15</v>
       </c>
@@ -2667,7 +2657,7 @@
         <f aca="false">IF(I46="Incerto",MAX(G46,J46-(ABS(F46*J46))),J46)</f>
         <v>0.0166666666666667</v>
       </c>
-      <c r="D46" s="5" t="n">
+      <c r="D46" s="2" t="n">
         <f aca="false">IF(I46="Incerto",MIN(H46,J46+(ABS(F46*J46))),J46)</f>
         <v>0.05</v>
       </c>
@@ -2708,7 +2698,7 @@
         <f aca="false">IF(I47="Incerto",MAX(G47,J47-(ABS(F47*J47))),J47)</f>
         <v>0</v>
       </c>
-      <c r="D47" s="5" t="n">
+      <c r="D47" s="2" t="n">
         <f aca="false">IF(I47="Incerto",MIN(H47,J47+(ABS(F47*J47))),J47)</f>
         <v>0</v>
       </c>
@@ -2744,7 +2734,7 @@
         <f aca="false">IF(I48="Incerto",MAX(G48,J48-(ABS(F48*J48))),J48)</f>
         <v>10</v>
       </c>
-      <c r="D48" s="5" t="n">
+      <c r="D48" s="2" t="n">
         <f aca="false">IF(I48="Incerto",MIN(H48,J48+(ABS(F48*J48))),J48)</f>
         <v>10</v>
       </c>
@@ -2778,7 +2768,7 @@
         <f aca="false">IF(I49="Incerto",MAX(G49,J49-(ABS(F49*J49))),J49)</f>
         <v>-6</v>
       </c>
-      <c r="D49" s="5" t="n">
+      <c r="D49" s="2" t="n">
         <f aca="false">IF(I49="Incerto",MIN(H49,J49+(ABS(F49*J49))),J49)</f>
         <v>-2</v>
       </c>
@@ -2810,7 +2800,7 @@
         <f aca="false">IF(I50="Incerto",MAX(G50,J50-(ABS(F50*J50))),J50)</f>
         <v>10</v>
       </c>
-      <c r="D50" s="5" t="n">
+      <c r="D50" s="2" t="n">
         <f aca="false">IF(I50="Incerto",MIN(H50,J50+(ABS(F50*J50))),J50)</f>
         <v>10</v>
       </c>
@@ -2844,7 +2834,7 @@
         <f aca="false">IF(I51="Incerto",MAX(G51,J51-(ABS(F51*J51))),J51)</f>
         <v>500</v>
       </c>
-      <c r="D51" s="5" t="n">
+      <c r="D51" s="2" t="n">
         <f aca="false">IF(I51="Incerto",MIN(H51,J51+(ABS(F51*J51))),J51)</f>
         <v>1500</v>
       </c>
@@ -2878,7 +2868,7 @@
         <f aca="false">IF(I52="Incerto",MAX(G52,J52-(ABS(F52*J52))),J52)</f>
         <v>50</v>
       </c>
-      <c r="D52" s="5" t="n">
+      <c r="D52" s="2" t="n">
         <f aca="false">IF(I52="Incerto",MIN(H52,J52+(ABS(F52*J52))),J52)</f>
         <v>150</v>
       </c>
@@ -2912,7 +2902,7 @@
         <f aca="false">IF(I53="Incerto",MAX(G53,J53-(ABS(F53*J53))),J53)</f>
         <v>50</v>
       </c>
-      <c r="D53" s="5" t="n">
+      <c r="D53" s="2" t="n">
         <f aca="false">IF(I53="Incerto",MIN(H53,J53+(ABS(F53*J53))),J53)</f>
         <v>150</v>
       </c>
@@ -2946,7 +2936,7 @@
         <f aca="false">IF(I54="Incerto",MAX(G54,J54-(ABS(F54*J54))),J54)</f>
         <v>10</v>
       </c>
-      <c r="D54" s="5" t="n">
+      <c r="D54" s="2" t="n">
         <f aca="false">IF(I54="Incerto",MIN(H54,J54+(ABS(F54*J54))),J54)</f>
         <v>30</v>
       </c>
@@ -2980,7 +2970,7 @@
         <f aca="false">IF(I55="Incerto",MAX(G55,J55-(ABS(F55*J55))),J55)</f>
         <v>500000</v>
       </c>
-      <c r="D55" s="5" t="n">
+      <c r="D55" s="2" t="n">
         <f aca="false">IF(I55="Incerto",MIN(H55,J55+(ABS(F55*J55))),J55)</f>
         <v>1500000</v>
       </c>
@@ -3016,7 +3006,7 @@
         <f aca="false">IF(I56="Incerto",MAX(G56,J56-(ABS(F56*J56))),J56)</f>
         <v>0.5</v>
       </c>
-      <c r="D56" s="5" t="n">
+      <c r="D56" s="2" t="n">
         <f aca="false">IF(I56="Incerto",MIN(H56,J56+(ABS(F56*J56))),J56)</f>
         <v>0.5</v>
       </c>
@@ -3065,11 +3055,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.32142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.1938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="4.18367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="7.29081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3125,11 +3115,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>136</v>
       </c>
       <c r="B1" s="0" t="s">
@@ -3174,11 +3164,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>